<commit_message>
Added product landing slide 10 and 14 URLs for all the 9 locales.
</commit_message>
<xml_diff>
--- a/docs/OVWDemo.xlsx
+++ b/docs/OVWDemo.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\OVWMigration\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="375" windowWidth="19410" windowHeight="9225" activeTab="8"/>
   </bookViews>
@@ -12,9 +17,9 @@
     <sheet name="zh_cn" sheetId="18" r:id="rId3"/>
     <sheet name="ru_ru" sheetId="10" r:id="rId4"/>
     <sheet name="pt_pt" sheetId="11" r:id="rId5"/>
-    <sheet name="es_es" sheetId="12" r:id="rId6"/>
-    <sheet name="ar_ae" sheetId="13" r:id="rId7"/>
-    <sheet name="fr_fr" sheetId="15" r:id="rId8"/>
+    <sheet name="ar_ae" sheetId="13" r:id="rId6"/>
+    <sheet name="fr_fr" sheetId="15" r:id="rId7"/>
+    <sheet name="es_es" sheetId="12" r:id="rId8"/>
     <sheet name="en_au" sheetId="16" r:id="rId9"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="127">
   <si>
     <t>index-var2</t>
   </si>
@@ -346,6 +351,63 @@
   </si>
   <si>
     <t>http://www.cisco.com/web/ANZ/products/voice/benefits.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/DE/solutions/datacenter/index.html</t>
+  </si>
+  <si>
+    <t>index-var10</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/DE/solutions/collaboration/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/JP/solution/datacenter/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/JP/solution/collaboration/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CN/solutions/collaboration/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/RU/solutions/collaboration/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/PT/solutions/collaboration/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ME/ar/solutions/collaboration/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/FR/solutions/collaboration/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ES/solutions/collaboration/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ANZ/netsol/collaboration/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ANZ/netsol/datacenter/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ES/solutions/datacenter/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/FR/solutions/datacenter/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ME/ar/solutions/datacenter/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/PT/solutions/datacenter/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/RU/solutions/datacenter/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CN/solutions/datacenter/index.html</t>
   </si>
 </sst>
 </file>
@@ -493,7 +555,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -528,7 +590,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -737,16 +799,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="61.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="15.42578125" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" customWidth="1"/>
   </cols>
@@ -889,6 +951,34 @@
       </c>
       <c r="D10" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" t="s">
+        <v>109</v>
+      </c>
+      <c r="D11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" t="s">
+        <v>109</v>
+      </c>
+      <c r="D12" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -903,18 +993,20 @@
     <hyperlink ref="A9" r:id="rId8"/>
     <hyperlink ref="A10" r:id="rId9"/>
     <hyperlink ref="A8" r:id="rId10"/>
+    <hyperlink ref="A11" r:id="rId11"/>
+    <hyperlink ref="A12" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:D9"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1050,6 +1142,34 @@
         <v>1</v>
       </c>
     </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" t="s">
+        <v>109</v>
+      </c>
+      <c r="D11" t="s">
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>
@@ -1061,6 +1181,8 @@
     <hyperlink ref="A7" r:id="rId7"/>
     <hyperlink ref="A8" r:id="rId8"/>
     <hyperlink ref="A9" r:id="rId9"/>
+    <hyperlink ref="A10" r:id="rId10"/>
+    <hyperlink ref="A11" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1068,10 +1190,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:D9"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1207,6 +1329,34 @@
         <v>1</v>
       </c>
     </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" t="s">
+        <v>109</v>
+      </c>
+      <c r="D11" t="s">
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>
@@ -1218,6 +1368,8 @@
     <hyperlink ref="A7" r:id="rId7"/>
     <hyperlink ref="A8" r:id="rId8"/>
     <hyperlink ref="A9" r:id="rId9"/>
+    <hyperlink ref="A11" r:id="rId10"/>
+    <hyperlink ref="A10" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1225,10 +1377,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:D10"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1379,6 +1531,34 @@
         <v>1</v>
       </c>
     </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" t="s">
+        <v>109</v>
+      </c>
+      <c r="D11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" t="s">
+        <v>109</v>
+      </c>
+      <c r="D12" t="s">
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>
@@ -1391,6 +1571,8 @@
     <hyperlink ref="A8" r:id="rId8"/>
     <hyperlink ref="A9" r:id="rId9"/>
     <hyperlink ref="A10" r:id="rId10"/>
+    <hyperlink ref="A12" r:id="rId11"/>
+    <hyperlink ref="A11" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1398,10 +1580,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:D10"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1552,6 +1734,34 @@
         <v>1</v>
       </c>
     </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" t="s">
+        <v>109</v>
+      </c>
+      <c r="D11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" t="s">
+        <v>109</v>
+      </c>
+      <c r="D12" t="s">
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>
@@ -1564,6 +1774,8 @@
     <hyperlink ref="A8" r:id="rId8"/>
     <hyperlink ref="A9" r:id="rId9"/>
     <hyperlink ref="A10" r:id="rId10"/>
+    <hyperlink ref="A12" r:id="rId11"/>
+    <hyperlink ref="A11" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1571,10 +1783,416 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:D10"/>
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="68.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" t="s">
+        <v>109</v>
+      </c>
+      <c r="D11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" t="s">
+        <v>109</v>
+      </c>
+      <c r="D12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId2"/>
+    <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A4" r:id="rId4"/>
+    <hyperlink ref="A5" r:id="rId5"/>
+    <hyperlink ref="A6" r:id="rId6"/>
+    <hyperlink ref="A7" r:id="rId7"/>
+    <hyperlink ref="A8" r:id="rId8"/>
+    <hyperlink ref="A9" r:id="rId9"/>
+    <hyperlink ref="A10" r:id="rId10"/>
+    <hyperlink ref="A12" r:id="rId11"/>
+    <hyperlink ref="A11" r:id="rId12"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="68.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" t="s">
+        <v>109</v>
+      </c>
+      <c r="D11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" t="s">
+        <v>109</v>
+      </c>
+      <c r="D12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId2"/>
+    <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A4" r:id="rId4"/>
+    <hyperlink ref="A5" r:id="rId5"/>
+    <hyperlink ref="A6" r:id="rId6"/>
+    <hyperlink ref="A7" r:id="rId7"/>
+    <hyperlink ref="A8" r:id="rId8"/>
+    <hyperlink ref="A9" r:id="rId9"/>
+    <hyperlink ref="A10" r:id="rId10"/>
+    <hyperlink ref="A12" r:id="rId11"/>
+    <hyperlink ref="A11" r:id="rId12"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1725,6 +2343,34 @@
         <v>1</v>
       </c>
     </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" t="s">
+        <v>109</v>
+      </c>
+      <c r="D11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" t="s">
+        <v>109</v>
+      </c>
+      <c r="D12" t="s">
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>
@@ -1737,30 +2383,32 @@
     <hyperlink ref="A8" r:id="rId8"/>
     <hyperlink ref="A9" r:id="rId9"/>
     <hyperlink ref="A10" r:id="rId10"/>
+    <hyperlink ref="A12" r:id="rId11"/>
+    <hyperlink ref="A11" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="68.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="67.140625" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -1773,8 +2421,8 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>26</v>
+      <c r="A2" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -1787,8 +2435,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>34</v>
+      <c r="A3" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
@@ -1801,8 +2449,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>42</v>
+      <c r="A4" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -1816,7 +2464,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
         <v>46</v>
@@ -1829,8 +2477,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>93</v>
+      <c r="A6" s="3" t="s">
+        <v>103</v>
       </c>
       <c r="B6" t="s">
         <v>57</v>
@@ -1844,7 +2492,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="B7" t="s">
         <v>60</v>
@@ -1858,7 +2506,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>64</v>
@@ -1872,7 +2520,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>67</v>
@@ -1886,7 +2534,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="B10" t="s">
         <v>69</v>
@@ -1896,6 +2544,34 @@
       </c>
       <c r="D10" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" t="s">
+        <v>109</v>
+      </c>
+      <c r="D11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" t="s">
+        <v>109</v>
+      </c>
+      <c r="D12" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1910,352 +2586,8 @@
     <hyperlink ref="A8" r:id="rId8"/>
     <hyperlink ref="A9" r:id="rId9"/>
     <hyperlink ref="A10" r:id="rId10"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:D10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="68.42578125" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="B6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="C8" t="s">
-        <v>65</v>
-      </c>
-      <c r="D8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C9" t="s">
-        <v>65</v>
-      </c>
-      <c r="D9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="B10" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" t="s">
-        <v>65</v>
-      </c>
-      <c r="D10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1"/>
-    <hyperlink ref="A2" r:id="rId2"/>
-    <hyperlink ref="A3" r:id="rId3"/>
-    <hyperlink ref="A4" r:id="rId4"/>
-    <hyperlink ref="A5" r:id="rId5"/>
-    <hyperlink ref="A6" r:id="rId6"/>
-    <hyperlink ref="A7" r:id="rId7"/>
-    <hyperlink ref="A8" r:id="rId8"/>
-    <hyperlink ref="A9" r:id="rId9"/>
-    <hyperlink ref="A10" r:id="rId10"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="67.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="C8" t="s">
-        <v>65</v>
-      </c>
-      <c r="D8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C9" t="s">
-        <v>65</v>
-      </c>
-      <c r="D9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="B10" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" t="s">
-        <v>65</v>
-      </c>
-      <c r="D10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1"/>
-    <hyperlink ref="A2" r:id="rId2"/>
-    <hyperlink ref="A3" r:id="rId3"/>
-    <hyperlink ref="A4" r:id="rId4"/>
-    <hyperlink ref="A5" r:id="rId5"/>
-    <hyperlink ref="A6" r:id="rId6"/>
-    <hyperlink ref="A7" r:id="rId7"/>
-    <hyperlink ref="A8" r:id="rId8"/>
-    <hyperlink ref="A9" r:id="rId9"/>
-    <hyperlink ref="A10" r:id="rId10"/>
+    <hyperlink ref="A12" r:id="rId11"/>
+    <hyperlink ref="A11" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated code for the variation 5 and 6.
</commit_message>
<xml_diff>
--- a/docs/OVWDemo.xlsx
+++ b/docs/OVWDemo.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\OVWMigration\docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="375" windowWidth="19410" windowHeight="9225" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="372" windowWidth="19416" windowHeight="9228" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="de_de" sheetId="2" r:id="rId1"/>
@@ -27,10 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="127">
-  <si>
-    <t>index-var2</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="128">
   <si>
     <t>products</t>
   </si>
@@ -408,6 +400,12 @@
   </si>
   <si>
     <t>http://www.cisco.com/web/CN/solutions/datacenter/index.html</t>
+  </si>
+  <si>
+    <t>index-var5</t>
+  </si>
+  <si>
+    <t>index-5</t>
   </si>
 </sst>
 </file>
@@ -555,7 +553,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -590,7 +588,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -799,186 +797,200 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="61.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="1" max="1" width="61.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.44140625" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>126</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
       <c r="D3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
       <c r="D4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" t="s">
         <v>45</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>46</v>
       </c>
-      <c r="C5" t="s">
-        <v>47</v>
-      </c>
       <c r="D5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" t="s">
         <v>56</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>57</v>
       </c>
-      <c r="C6" t="s">
-        <v>58</v>
-      </c>
       <c r="D6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" t="s">
         <v>59</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>60</v>
       </c>
-      <c r="C7" t="s">
-        <v>61</v>
-      </c>
       <c r="D7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="C8" t="s">
         <v>64</v>
       </c>
-      <c r="C8" t="s">
-        <v>65</v>
-      </c>
       <c r="D8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>67</v>
-      </c>
       <c r="C9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" t="s">
         <v>68</v>
       </c>
-      <c r="B10" t="s">
-        <v>69</v>
-      </c>
       <c r="C10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D10" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" t="s">
         <v>108</v>
       </c>
-      <c r="B11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C11" t="s">
-        <v>109</v>
-      </c>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D12" t="s">
-        <v>62</v>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1006,168 +1018,168 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="62.5703125" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" customWidth="1"/>
+    <col min="1" max="1" width="62.5546875" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>126</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
       <c r="D3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
       <c r="D4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
         <v>46</v>
       </c>
-      <c r="C5" t="s">
-        <v>47</v>
-      </c>
       <c r="D5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" t="s">
         <v>57</v>
       </c>
-      <c r="C6" t="s">
-        <v>58</v>
-      </c>
       <c r="D6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B7" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" t="s">
         <v>64</v>
       </c>
-      <c r="C7" t="s">
-        <v>65</v>
-      </c>
       <c r="D7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D9" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1193,168 +1205,168 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="81.5703125" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="81.5546875" customWidth="1"/>
+    <col min="2" max="2" width="23.109375" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>126</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
       <c r="D3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
       <c r="D4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
         <v>46</v>
       </c>
-      <c r="C5" t="s">
-        <v>47</v>
-      </c>
       <c r="D5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" t="s">
         <v>57</v>
       </c>
-      <c r="C6" t="s">
-        <v>58</v>
-      </c>
       <c r="D6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B7" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" t="s">
         <v>64</v>
       </c>
-      <c r="C7" t="s">
-        <v>65</v>
-      </c>
       <c r="D7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D9" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1379,184 +1391,184 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="66.28515625" customWidth="1"/>
+    <col min="1" max="1" width="66.33203125" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>126</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
       <c r="D3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
       <c r="D4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
         <v>46</v>
       </c>
-      <c r="C5" t="s">
-        <v>47</v>
-      </c>
       <c r="D5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" t="s">
         <v>57</v>
       </c>
-      <c r="C6" t="s">
-        <v>58</v>
-      </c>
       <c r="D6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" t="s">
         <v>60</v>
       </c>
-      <c r="C7" t="s">
-        <v>61</v>
-      </c>
       <c r="D7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B8" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" t="s">
         <v>64</v>
       </c>
-      <c r="C8" t="s">
-        <v>65</v>
-      </c>
       <c r="D8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D10" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1583,183 +1595,183 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="67.140625" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="67.109375" customWidth="1"/>
+    <col min="2" max="2" width="23.109375" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
       <c r="D3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
       <c r="D4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
         <v>46</v>
       </c>
-      <c r="C5" t="s">
-        <v>47</v>
-      </c>
       <c r="D5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" t="s">
         <v>57</v>
       </c>
-      <c r="C6" t="s">
-        <v>58</v>
-      </c>
       <c r="D6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" t="s">
         <v>60</v>
       </c>
-      <c r="C7" t="s">
-        <v>61</v>
-      </c>
       <c r="D7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B8" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" t="s">
         <v>64</v>
       </c>
-      <c r="C8" t="s">
-        <v>65</v>
-      </c>
       <c r="D8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D10" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1786,183 +1798,183 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="68.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" customWidth="1"/>
+    <col min="1" max="1" width="68.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.109375" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>126</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
       <c r="D3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
       <c r="D4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
         <v>46</v>
       </c>
-      <c r="C5" t="s">
-        <v>47</v>
-      </c>
       <c r="D5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" t="s">
         <v>57</v>
       </c>
-      <c r="C6" t="s">
-        <v>58</v>
-      </c>
       <c r="D6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" t="s">
         <v>60</v>
       </c>
-      <c r="C7" t="s">
-        <v>61</v>
-      </c>
       <c r="D7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B8" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" t="s">
         <v>64</v>
       </c>
-      <c r="C8" t="s">
-        <v>65</v>
-      </c>
       <c r="D8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D10" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1989,183 +2001,183 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="68.42578125" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="68.44140625" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>126</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
       <c r="D3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
       <c r="D4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
         <v>46</v>
       </c>
-      <c r="C5" t="s">
-        <v>47</v>
-      </c>
       <c r="D5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" t="s">
         <v>57</v>
       </c>
-      <c r="C6" t="s">
-        <v>58</v>
-      </c>
       <c r="D6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" t="s">
         <v>60</v>
       </c>
-      <c r="C7" t="s">
-        <v>61</v>
-      </c>
       <c r="D7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B8" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" t="s">
         <v>64</v>
       </c>
-      <c r="C8" t="s">
-        <v>65</v>
-      </c>
       <c r="D8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D10" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -2192,183 +2204,183 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="69.140625" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="1" max="1" width="69.109375" customWidth="1"/>
+    <col min="2" max="2" width="26.5546875" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>126</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
       <c r="D3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
       <c r="D4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
         <v>46</v>
       </c>
-      <c r="C5" t="s">
-        <v>47</v>
-      </c>
       <c r="D5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" t="s">
         <v>57</v>
       </c>
-      <c r="C6" t="s">
-        <v>58</v>
-      </c>
       <c r="D6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" t="s">
         <v>60</v>
       </c>
-      <c r="C7" t="s">
-        <v>61</v>
-      </c>
       <c r="D7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B8" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" t="s">
         <v>64</v>
       </c>
-      <c r="C8" t="s">
-        <v>65</v>
-      </c>
       <c r="D8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D10" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -2394,184 +2406,184 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="67.140625" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="1" max="1" width="67.109375" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>126</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
       <c r="D3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
       <c r="D4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
         <v>46</v>
       </c>
-      <c r="C5" t="s">
-        <v>47</v>
-      </c>
       <c r="D5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" t="s">
         <v>57</v>
       </c>
-      <c r="C6" t="s">
-        <v>58</v>
-      </c>
       <c r="D6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" t="s">
         <v>60</v>
       </c>
-      <c r="C7" t="s">
-        <v>61</v>
-      </c>
       <c r="D7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B8" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" t="s">
         <v>64</v>
       </c>
-      <c r="C8" t="s">
-        <v>65</v>
-      </c>
       <c r="D8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D10" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>